<commit_message>
fucking around in the rmd
</commit_message>
<xml_diff>
--- a/emd538/problem-sets/ps1/EMD538_2023_Lab2_Blank.xlsx
+++ b/emd538/problem-sets/ps1/EMD538_2023_Lab2_Blank.xlsx
@@ -1,24 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mailealmostphillips/Desktop/EMD538/Lab/Lab2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colebrookson/github/fall-courses-2024/emd538/problem-sets/ps1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E570C31A-CC8D-0940-9A8F-7BEA7193C201}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7CB564-C78B-4F49-8AAB-27E83A0EA96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10460" yWindow="460" windowWidth="18340" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10460" yWindow="760" windowWidth="18340" windowHeight="16020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -100,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -376,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -389,13 +399,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -415,7 +421,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -425,7 +431,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -811,11 +816,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
@@ -823,56 +828,56 @@
     <col min="14" max="14" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="25"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="L1" s="23"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="37" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="M3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="43" t="s">
+      <c r="N3" s="40" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="35"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="44"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+    <row r="4" spans="1:14">
+      <c r="A4" s="32"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="41"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="33"/>
       <c r="B5" s="3">
         <v>1</v>
       </c>
@@ -903,11 +908,11 @@
       <c r="K5" s="7">
         <v>10</v>
       </c>
-      <c r="L5" s="39"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="44"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L5" s="36"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="41"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="4">
         <v>0</v>
       </c>
@@ -941,11 +946,17 @@
       <c r="K6" s="8">
         <v>0</v>
       </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="29"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L6" s="12">
+        <f>SUM(B6:K6)</f>
+        <v>723</v>
+      </c>
+      <c r="M6" s="25">
+        <f>L6*A6</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="26"/>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -979,11 +990,17 @@
       <c r="K7" s="8">
         <v>0</v>
       </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="30"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L7" s="12">
+        <f t="shared" ref="L7:L15" si="0">SUM(B7:K7)</f>
+        <v>384</v>
+      </c>
+      <c r="M7" s="25">
+        <f t="shared" ref="M7:M13" si="1">L7*A7</f>
+        <v>384</v>
+      </c>
+      <c r="N7" s="27"/>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="5">
         <v>2</v>
       </c>
@@ -1017,11 +1034,17 @@
       <c r="K8" s="8">
         <v>1</v>
       </c>
-      <c r="L8" s="13"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="30"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L8" s="12">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="M8" s="25">
+        <f t="shared" si="1"/>
+        <v>312</v>
+      </c>
+      <c r="N8" s="27"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="5">
         <v>3</v>
       </c>
@@ -1055,11 +1078,17 @@
       <c r="K9" s="8">
         <v>0</v>
       </c>
-      <c r="L9" s="13"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="30"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L9" s="12">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="M9" s="25">
+        <f t="shared" si="1"/>
+        <v>171</v>
+      </c>
+      <c r="N9" s="27"/>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="5">
         <v>4</v>
       </c>
@@ -1093,11 +1122,17 @@
       <c r="K10" s="8">
         <v>0</v>
       </c>
-      <c r="L10" s="13"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="13"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L10" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M10" s="25">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="N10" s="12"/>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="5">
         <v>5</v>
       </c>
@@ -1131,11 +1166,17 @@
       <c r="K11" s="8">
         <v>0</v>
       </c>
-      <c r="L11" s="13"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="13"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L11" s="12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M11" s="25">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="N11" s="12"/>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="5">
         <v>6</v>
       </c>
@@ -1169,11 +1210,17 @@
       <c r="K12" s="8">
         <v>0</v>
       </c>
-      <c r="L12" s="13"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="13"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L12" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M12" s="25">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="N12" s="12"/>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="6">
         <v>7</v>
       </c>
@@ -1207,32 +1254,38 @@
       <c r="K13" s="9">
         <v>0</v>
       </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="14"/>
-    </row>
-    <row r="14" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
+      <c r="L13" s="12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M13" s="25">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="N13" s="13"/>
+    </row>
+    <row r="14" spans="1:14" ht="32">
+      <c r="A14" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15">
-        <f t="shared" ref="M14" si="0">SUM(M6:M13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="14">
+        <f>SUM(M6:M13)</f>
+        <v>952</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="32">
+      <c r="A15" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="10"/>
@@ -1245,50 +1298,50 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="9"/>
-      <c r="L15" s="11"/>
+      <c r="L15" s="12"/>
       <c r="M15" s="11"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" s="17"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="18"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="22" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" s="19"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="18" t="s">
+    <row r="23" spans="1:1">
+      <c r="A23" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
+    <row r="24" spans="1:1">
+      <c r="A24" s="17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
+    <row r="26" spans="1:1">
+      <c r="A26" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="23"/>
+    <row r="27" spans="1:1">
+      <c r="A27" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>